<commit_message>
Add people to recovered compartment to avoid -ve people error
</commit_message>
<xml_diff>
--- a/tests/cascade_spreadsheet/cascade_model_simple.xlsx
+++ b/tests/cascade_spreadsheet/cascade_model_simple.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14445" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14445" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="105">
   <si>
     <t>Code Label</t>
   </si>
@@ -335,6 +335,9 @@
   </si>
   <si>
     <t>Deaths</t>
+  </si>
+  <si>
+    <t>rec_label</t>
   </si>
 </sst>
 </file>
@@ -1025,10 +1028,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1317,6 +1320,32 @@
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" s="10"/>
+      <c r="E11" s="8">
+        <v>5000</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="9"/>
+      <c r="I11" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J11" s="7"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1623,7 +1652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>